<commit_message>
UX e CSS menor
-cabeçalhos melhorados
</commit_message>
<xml_diff>
--- a/umbrella360/deposito/relatorio_[UMBR]INFRA.xlsx
+++ b/umbrella360/deposito/relatorio_[UMBR]INFRA.xlsx
@@ -584,12 +584,12 @@
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>7:51:26</t>
+          <t>8:19:06</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>14 days 5:40:41</t>
+          <t>16 days 2:25:52</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
@@ -604,7 +604,7 @@
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>99 km/h</t>
+          <t>98 km/h</t>
         </is>
       </c>
       <c r="L3" t="inlineStr">
@@ -647,12 +647,12 @@
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>1:06:46</t>
+          <t>1:08:38</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>7 days 13:44:07</t>
+          <t>15 days 23:57:35</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
@@ -667,7 +667,7 @@
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>105 km/h</t>
+          <t>104 km/h</t>
         </is>
       </c>
       <c r="L4" t="inlineStr">
@@ -765,12 +765,12 @@
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>0:01:29</t>
+          <t>0:02:06</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>4 days 0:29:05</t>
+          <t>5 days 23:22:38</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
@@ -785,7 +785,7 @@
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>73 km/h</t>
+          <t>71 km/h</t>
         </is>
       </c>
       <c r="L6" t="inlineStr">
@@ -887,12 +887,12 @@
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>6:20:33</t>
+          <t>7:15:59</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>27 days 8:40:35</t>
+          <t>29 days 1:34:17</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
@@ -907,7 +907,7 @@
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>112 km/h</t>
+          <t>109 km/h</t>
         </is>
       </c>
       <c r="L8" t="inlineStr">
@@ -950,12 +950,12 @@
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>17:03:55</t>
+          <t>17:30:43</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>24 days 11:34:36</t>
+          <t>26 days 11:24:20</t>
         </is>
       </c>
       <c r="I9" t="inlineStr">
@@ -997,28 +997,28 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>21.07.2025 14:54:23</t>
+          <t>22.07.2025 11:05:52</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Rua Mun. City Ribeirão, Ribeirão Preto, SP 14000-000, Brazil</t>
+          <t>55B, Subsetor Leste-6, Ribeirão Preto, SP, Brazil</t>
         </is>
       </c>
       <c r="E10" t="n">
-        <v>-21.2254366</v>
+        <v>-21.2048116</v>
       </c>
       <c r="F10" t="n">
-        <v>-47.75549</v>
+        <v>-47.757315</v>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>3:58:19</t>
+          <t>3:50:01</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>23 days 0:40:25</t>
+          <t>22 days 4:28:56</t>
         </is>
       </c>
       <c r="I10" t="inlineStr">
@@ -1028,7 +1028,7 @@
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>63 km/h</t>
+          <t>75 km/h</t>
         </is>
       </c>
       <c r="K10" t="inlineStr">
@@ -1038,7 +1038,7 @@
       </c>
       <c r="L10" t="inlineStr">
         <is>
-          <t>50 km/h</t>
+          <t>40 km/h</t>
         </is>
       </c>
       <c r="M10" t="inlineStr">
@@ -1076,12 +1076,12 @@
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>5:46:32</t>
+          <t>5:57:58</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>26 days 21:51:58</t>
+          <t>29 days 5:49:33</t>
         </is>
       </c>
       <c r="I11" t="inlineStr">
@@ -1096,7 +1096,7 @@
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>116 km/h</t>
+          <t>115 km/h</t>
         </is>
       </c>
       <c r="L11" t="inlineStr">
@@ -1186,28 +1186,28 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>21.07.2025 14:25:13</t>
+          <t>22.07.2025 08:51:55</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>Mg-427, Conceição Das Alagoas, MG 38120-000, Brazil</t>
+          <t>Sp-328, Ribeirão Preto, SP, Brazil</t>
         </is>
       </c>
       <c r="E13" t="n">
-        <v>-19.972705</v>
+        <v>-21.0958533</v>
       </c>
       <c r="F13" t="n">
-        <v>-48.3080583</v>
+        <v>-47.7963533</v>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>15:20:55</t>
+          <t>14:06:15</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>25 days 3:13:40</t>
+          <t>27 days 12:17:06</t>
         </is>
       </c>
       <c r="I13" t="inlineStr">
@@ -1217,7 +1217,7 @@
       </c>
       <c r="J13" t="inlineStr">
         <is>
-          <t>123 km/h</t>
+          <t>102 km/h</t>
         </is>
       </c>
       <c r="K13" t="inlineStr">
@@ -1261,12 +1261,12 @@
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>4:45:42</t>
+          <t>4:46:32</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>8 days 21:38:15</t>
+          <t>9 days 23:44:22</t>
         </is>
       </c>
       <c r="I14" t="inlineStr">
@@ -1320,12 +1320,12 @@
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>6:52:51</t>
+          <t>8:09:02</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>12 days 5:38:35</t>
+          <t>13 days 7:06:23</t>
         </is>
       </c>
       <c r="I15" t="inlineStr">
@@ -1383,12 +1383,12 @@
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>11:47:47</t>
+          <t>13:11:34</t>
         </is>
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>20 days 1:13:01</t>
+          <t>22 days 2:32:33</t>
         </is>
       </c>
       <c r="I16" t="inlineStr">
@@ -1489,43 +1489,43 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>21.07.2025 15:59:00</t>
+          <t>22.07.2025 10:06:50</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>Rodovia Attílio Balbo, Sertãozinho, SP 14173-000, Brazil</t>
+          <t>Avenida Gen. Euclydes De Figueiredo, Subsetor Norte-10, Ribeirão Preto, SP 14070-270, Brazil</t>
         </is>
       </c>
       <c r="E18" t="n">
-        <v>-21.167295</v>
+        <v>-21.1112716</v>
       </c>
       <c r="F18" t="n">
-        <v>-47.9179833</v>
+        <v>-47.790145</v>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>12:23:50</t>
+          <t>14:36:40</t>
         </is>
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>25 days 3:09:47</t>
+          <t>29 days 6:21:20</t>
         </is>
       </c>
       <c r="I18" t="inlineStr">
         <is>
-          <t>{'t': '139 km/h', 'y': -21.6998983, 'x': -48.0234933, 'u': 401879415}</t>
+          <t>{'t': '140 km/h', 'y': -20.4904, 'x': -42.1855633, 'u': 401879415}</t>
         </is>
       </c>
       <c r="J18" t="inlineStr">
         <is>
-          <t>74 km/h</t>
+          <t>54 km/h</t>
         </is>
       </c>
       <c r="K18" t="inlineStr">
         <is>
-          <t>94 km/h</t>
+          <t>93 km/h</t>
         </is>
       </c>
       <c r="L18" t="inlineStr">
@@ -1564,12 +1564,12 @@
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>12:31:08</t>
+          <t>14:49:57</t>
         </is>
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>12 days 7:51:15</t>
+          <t>14 days 8:57:10</t>
         </is>
       </c>
       <c r="I19" t="inlineStr">
@@ -1584,7 +1584,7 @@
       </c>
       <c r="K19" t="inlineStr">
         <is>
-          <t>107 km/h</t>
+          <t>106 km/h</t>
         </is>
       </c>
       <c r="L19" t="inlineStr">
@@ -1627,12 +1627,12 @@
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>6:41:19</t>
+          <t>7:03:02</t>
         </is>
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>20 days 19:32:14</t>
+          <t>26 days 5:35:52</t>
         </is>
       </c>
       <c r="I20" t="inlineStr">
@@ -1647,7 +1647,7 @@
       </c>
       <c r="K20" t="inlineStr">
         <is>
-          <t>106 km/h</t>
+          <t>105 km/h</t>
         </is>
       </c>
       <c r="L20" t="inlineStr">
@@ -1686,12 +1686,12 @@
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>7:22:55</t>
+          <t>8:27:11</t>
         </is>
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>12 days 9:04:55</t>
+          <t>14 days 6:37:00</t>
         </is>
       </c>
       <c r="I21" t="inlineStr">
@@ -1749,12 +1749,12 @@
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>7:28:13</t>
+          <t>8:15:24</t>
         </is>
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>23 days 5:59:13</t>
+          <t>27 days 5:50:48</t>
         </is>
       </c>
       <c r="I22" t="inlineStr">
@@ -1769,7 +1769,7 @@
       </c>
       <c r="K22" t="inlineStr">
         <is>
-          <t>110 km/h</t>
+          <t>108 km/h</t>
         </is>
       </c>
       <c r="L22" t="inlineStr">
@@ -1812,12 +1812,12 @@
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>6:26:07</t>
+          <t>9:00:27</t>
         </is>
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>25 days 0:40:32</t>
+          <t>27 days 2:16:17</t>
         </is>
       </c>
       <c r="I23" t="inlineStr">
@@ -1832,7 +1832,7 @@
       </c>
       <c r="K23" t="inlineStr">
         <is>
-          <t>107 km/h</t>
+          <t>106 km/h</t>
         </is>
       </c>
       <c r="L23" t="inlineStr">
@@ -1871,17 +1871,17 @@
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>1:21:56</t>
+          <t>3:43:47</t>
         </is>
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>12 days 5:27:03</t>
+          <t>14 days 0:23:52</t>
         </is>
       </c>
       <c r="I24" t="inlineStr">
         <is>
-          <t>{'t': '146 km/h', 'y': -22.4994016, 'x': -49.2723066, 'u': 401929767}</t>
+          <t>{'t': '151 km/h', 'y': -22.6260566, 'x': -50.5993383, 'u': 401929767}</t>
         </is>
       </c>
       <c r="J24" t="inlineStr">
@@ -1891,7 +1891,7 @@
       </c>
       <c r="K24" t="inlineStr">
         <is>
-          <t>106 km/h</t>
+          <t>120 km/h</t>
         </is>
       </c>
       <c r="L24" t="inlineStr">
@@ -1930,12 +1930,12 @@
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>10:17:33</t>
+          <t>11:11:10</t>
         </is>
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>24 days 7:01:18</t>
+          <t>28 days 1:39:56</t>
         </is>
       </c>
       <c r="I25" t="inlineStr">
@@ -1950,7 +1950,7 @@
       </c>
       <c r="K25" t="inlineStr">
         <is>
-          <t>102 km/h</t>
+          <t>101 km/h</t>
         </is>
       </c>
       <c r="L25" t="inlineStr">
@@ -1993,12 +1993,12 @@
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>1:35:22</t>
+          <t>1:55:20</t>
         </is>
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>14 days 8:28:27</t>
+          <t>15 days 7:40:16</t>
         </is>
       </c>
       <c r="I26" t="inlineStr">
@@ -2056,12 +2056,12 @@
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>4:28:55</t>
+          <t>5:43:01</t>
         </is>
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>25 days 0:16:14</t>
+          <t>26 days 22:59:33</t>
         </is>
       </c>
       <c r="I27" t="inlineStr">
@@ -2115,17 +2115,17 @@
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>8:26:37</t>
+          <t>12:54:19</t>
         </is>
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>18 days 10:05:29</t>
+          <t>26 days 2:25:13</t>
         </is>
       </c>
       <c r="I28" t="inlineStr">
         <is>
-          <t>{'t': '184 km/h', 'y': -21.758285, 'x': -48.07348, 'u': 401897329}</t>
+          <t>{'t': '189 km/h', 'y': -21.7579216, 'x': -48.0730216, 'u': 401897329}</t>
         </is>
       </c>
       <c r="J28" t="inlineStr">
@@ -2135,7 +2135,7 @@
       </c>
       <c r="K28" t="inlineStr">
         <is>
-          <t>119 km/h</t>
+          <t>123 km/h</t>
         </is>
       </c>
       <c r="L28" t="inlineStr">
@@ -2174,12 +2174,12 @@
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>5:55:12</t>
+          <t>6:47:54</t>
         </is>
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>23 days 19:27:51</t>
+          <t>28 days 2:13:18</t>
         </is>
       </c>
       <c r="I29" t="inlineStr">
@@ -2194,7 +2194,7 @@
       </c>
       <c r="K29" t="inlineStr">
         <is>
-          <t>114 km/h</t>
+          <t>112 km/h</t>
         </is>
       </c>
       <c r="L29" t="inlineStr">
@@ -2237,12 +2237,12 @@
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>11:22:57</t>
+          <t>14:47:22</t>
         </is>
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>14 days 15:08:45</t>
+          <t>20 days 19:51:41</t>
         </is>
       </c>
       <c r="I30" t="inlineStr">
@@ -2257,7 +2257,7 @@
       </c>
       <c r="K30" t="inlineStr">
         <is>
-          <t>90 km/h</t>
+          <t>93 km/h</t>
         </is>
       </c>
       <c r="L30" t="inlineStr">
@@ -2418,12 +2418,12 @@
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t>0:17:43</t>
+          <t>0:28:18</t>
         </is>
       </c>
       <c r="H33" t="inlineStr">
         <is>
-          <t>4 days 4:48:01</t>
+          <t>5 days 5:02:23</t>
         </is>
       </c>
       <c r="I33" t="inlineStr">
@@ -2438,7 +2438,7 @@
       </c>
       <c r="K33" t="inlineStr">
         <is>
-          <t>87 km/h</t>
+          <t>88 km/h</t>
         </is>
       </c>
       <c r="L33" t="inlineStr">
@@ -2481,12 +2481,12 @@
       </c>
       <c r="G34" t="inlineStr">
         <is>
-          <t>5:17:25</t>
+          <t>5:22:00</t>
         </is>
       </c>
       <c r="H34" t="inlineStr">
         <is>
-          <t>25 days 0:59:02</t>
+          <t>27 days 0:57:28</t>
         </is>
       </c>
       <c r="I34" t="inlineStr">
@@ -2501,7 +2501,7 @@
       </c>
       <c r="K34" t="inlineStr">
         <is>
-          <t>114 km/h</t>
+          <t>113 km/h</t>
         </is>
       </c>
       <c r="L34" t="inlineStr">
@@ -2544,12 +2544,12 @@
       </c>
       <c r="G35" t="inlineStr">
         <is>
-          <t>10:48:38</t>
+          <t>16:29:00</t>
         </is>
       </c>
       <c r="H35" t="inlineStr">
         <is>
-          <t>24 days 13:33:10</t>
+          <t>27 days 2:37:47</t>
         </is>
       </c>
       <c r="I35" t="inlineStr">
@@ -2564,7 +2564,7 @@
       </c>
       <c r="K35" t="inlineStr">
         <is>
-          <t>106 km/h</t>
+          <t>105 km/h</t>
         </is>
       </c>
       <c r="L35" t="inlineStr">
@@ -2607,12 +2607,12 @@
       </c>
       <c r="G36" t="inlineStr">
         <is>
-          <t>11:08:10</t>
+          <t>15:11:47</t>
         </is>
       </c>
       <c r="H36" t="inlineStr">
         <is>
-          <t>11 days 5:24:20</t>
+          <t>15 days 13:48:18</t>
         </is>
       </c>
       <c r="I36" t="inlineStr">
@@ -2627,7 +2627,7 @@
       </c>
       <c r="K36" t="inlineStr">
         <is>
-          <t>103 km/h</t>
+          <t>104 km/h</t>
         </is>
       </c>
       <c r="L36" t="inlineStr">

</xml_diff>